<commit_message>
added Cat's phase codes
</commit_message>
<xml_diff>
--- a/FISH_MAN_namescrosswalk_20200122.xlsx
+++ b/FISH_MAN_namescrosswalk_20200122.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/North Delta Flow action/ND-FASTR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhartman\OneDrive - California Department of Water Resources\North Delta Flow action\ND-FASTR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="8_{214AFCD9-17CD-4B9B-9E13-D76600F86E8E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{3099AB64-CDA1-486C-8D78-75F41284AD74}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="8_{214AFCD9-17CD-4B9B-9E13-D76600F86E8E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{137CCC5C-763F-492C-BB01-2D9BA71CC1EA}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{954D08CE-A2BF-49C1-8AF9-792A340A95CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{954D08CE-A2BF-49C1-8AF9-792A340A95CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="300">
   <si>
     <t>CommonName</t>
   </si>
@@ -1284,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277204AF-F31C-42A6-8231-B2648801EB02}">
   <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,6 +1509,9 @@
       <c r="E7" t="s">
         <v>33</v>
       </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1881,6 +1884,9 @@
       <c r="E19" t="s">
         <v>290</v>
       </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2408,6 +2414,9 @@
       <c r="C35" t="s">
         <v>232</v>
       </c>
+      <c r="F35" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -2489,6 +2498,9 @@
       <c r="E38" t="s">
         <v>233</v>
       </c>
+      <c r="F38" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -2849,6 +2861,9 @@
       <c r="C50" t="s">
         <v>236</v>
       </c>
+      <c r="F50" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -2994,6 +3009,9 @@
       <c r="C55" t="s">
         <v>237</v>
       </c>
+      <c r="F55" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -3005,6 +3023,9 @@
       <c r="E56" t="s">
         <v>238</v>
       </c>
+      <c r="F56" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -3774,6 +3795,9 @@
       <c r="C79" t="s">
         <v>244</v>
       </c>
+      <c r="F79" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
@@ -3881,6 +3905,9 @@
       <c r="C83" t="s">
         <v>228</v>
       </c>
+      <c r="F83" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
@@ -3889,6 +3916,9 @@
       <c r="E84" t="s">
         <v>298</v>
       </c>
+      <c r="F84" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
@@ -3897,6 +3927,9 @@
       <c r="E85" t="s">
         <v>293</v>
       </c>
+      <c r="F85" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
@@ -3904,6 +3937,9 @@
       </c>
       <c r="E86" t="s">
         <v>292</v>
+      </c>
+      <c r="F86" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3916,6 +3952,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C65D496D98813D4DBEDE643E5807C583" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="47ba276ed79f27bd78102509b7910205">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="d8e3e477-4a6b-4f2c-bc61-5e11693be0f9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7cbb682bc36abf1978bf8322521ece19" ns1:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4102,25 +4156,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C24D1664-4FDC-4778-99E5-9EDACEFF3E08}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d8e3e477-4a6b-4f2c-bc61-5e11693be0f9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3633D6CF-EA3A-4FA7-BECE-ED6AD27EBC88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{340EB2BC-91DC-4E79-B1B1-C13B0F328630}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4137,29 +4198,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3633D6CF-EA3A-4FA7-BECE-ED6AD27EBC88}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C24D1664-4FDC-4778-99E5-9EDACEFF3E08}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d8e3e477-4a6b-4f2c-bc61-5e11693be0f9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>